<commit_message>
Prototyping and planning Room.java, as well as added a RoomTypes enum
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="16110" windowHeight="3210"/>
   </bookViews>
   <sheets>
     <sheet name="Victims" sheetId="1" r:id="rId1"/>
     <sheet name="Rooms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:Q11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>First Name</t>
   </si>
@@ -1198,146 +1199,145 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s" s="0">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s" s="0">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s" s="0">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="0"/>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:1">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated HotelRoom.java to interact with an Excel Spreadsheet. Modified Excel.java to acommodate. Other minor changes surrounding this.
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16110" windowHeight="3210"/>
+    <workbookView windowWidth="21000" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Victims" sheetId="1" r:id="rId1"/>
     <sheet name="Rooms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <oleSize ref="A1:Q11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>First Name</t>
   </si>
@@ -100,6 +99,36 @@
   </si>
   <si>
     <t>Ackerman</t>
+  </si>
+  <si>
+    <t>Room #</t>
+  </si>
+  <si>
+    <t>Check In</t>
+  </si>
+  <si>
+    <t>Check Out</t>
+  </si>
+  <si>
+    <t>2003-01-10</t>
+  </si>
+  <si>
+    <t>2003-01-15</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-28</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>300</t>
   </si>
 </sst>
 </file>
@@ -1199,145 +1228,145 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
@@ -1350,14 +1379,87 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AI4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="32:35">
+      <c r="A2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="AG2" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="AH2" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="AI2" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
handled handling of Customer personall info and some logic checking for Dates
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>First Name</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>300</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -1379,7 +1382,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI4"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1459,6 +1462,11 @@
         <v>37</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added methods to make sure reservations are chronological, and started functionality on room selection controller
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11730" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Victims" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>First Name</t>
   </si>
@@ -108,30 +108,6 @@
   </si>
   <si>
     <t>Check Out</t>
-  </si>
-  <si>
-    <t>2003-01-10</t>
-  </si>
-  <si>
-    <t>2003-01-15</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-28</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -1238,138 +1214,138 @@
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s" s="0">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s" s="0">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s" s="0">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="0">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="0">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="0">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="0">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s" s="0">
+      <c r="C5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="0">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="0">
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s" s="0">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" s="0">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="0">
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s" s="0">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
-      <c r="A8" s="0">
+      <c r="A8">
         <v>7</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
-      <c r="A9" s="0">
+      <c r="A9">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
-      <c r="A10" s="0">
+      <c r="A10">
         <v>9</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:1">
-      <c r="A11" s="0">
+      <c r="A11">
         <v>10</v>
       </c>
     </row>
@@ -1382,89 +1358,71 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
         <v>28</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="32:35">
-      <c r="A2" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
-      <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
-      <c r="Q2" s="0"/>
-      <c r="R2" s="0"/>
-      <c r="S2" s="0"/>
-      <c r="T2" s="0"/>
-      <c r="U2" s="0"/>
-      <c r="V2" s="0"/>
-      <c r="W2" s="0"/>
-      <c r="X2" s="0"/>
-      <c r="Y2" s="0"/>
-      <c r="Z2" s="0"/>
-      <c r="AA2" s="0"/>
-      <c r="AB2" s="0"/>
-      <c r="AC2" s="0"/>
-      <c r="AD2" s="0"/>
-      <c r="AE2" s="0"/>
-      <c r="AF2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="AG2" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="AH2" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="AI2" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>38</v>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got the Hotel Room class functioning, RoomSelection COntroller needs some work
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>First Name</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>Check Out</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -1358,13 +1361,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
@@ -1423,6 +1426,20 @@
       </c>
       <c r="S1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="32:35">
+      <c r="AF2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Room selection controller functionality
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>First Name</t>
   </si>
@@ -110,7 +110,43 @@
     <t>Check Out</t>
   </si>
   <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>2024-01-10</t>
+  </si>
+  <si>
+    <t>2024-01-15</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-28</t>
+  </si>
+  <si>
     <t/>
+  </si>
+  <si>
+    <t>2024-01-20</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>2023-01-10</t>
+  </si>
+  <si>
+    <t>2023-01-20</t>
   </si>
 </sst>
 </file>
@@ -1217,138 +1253,138 @@
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
@@ -1361,85 +1397,141 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" t="s" s="0">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="32:35">
-      <c r="AF2" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="AG2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>31</v>
+      <c r="B2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
+      <c r="Q2" s="0"/>
+      <c r="R2" s="0"/>
+      <c r="S2" s="0"/>
+      <c r="T2" s="0"/>
+      <c r="U2" s="0"/>
+      <c r="V2" s="0"/>
+      <c r="W2" s="0"/>
+      <c r="X2" s="0"/>
+      <c r="Y2" s="0"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Most up to date version 4/11
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="44">
   <si>
     <t>First Name</t>
   </si>
@@ -108,6 +108,45 @@
   </si>
   <si>
     <t>Check Out</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>2024-01-10</t>
+  </si>
+  <si>
+    <t>2024-01-15</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-28</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2024-01-20</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>2023-01-10</t>
+  </si>
+  <si>
+    <t>2023-01-20</t>
   </si>
 </sst>
 </file>
@@ -1214,138 +1253,138 @@
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:4">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:3">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:3">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>21</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:3">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:3">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>25</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:3">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>7</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>8</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>10</v>
       </c>
     </row>
@@ -1358,7 +1397,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:AU5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -1367,62 +1406,176 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" t="s" s="0">
         <v>30</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="Q2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="S2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="T2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="U2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="W2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="X2" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="Y2" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
+      <c r="AB2" s="0"/>
+      <c r="AC2" s="0"/>
+      <c r="AD2" s="0"/>
+      <c r="AE2" s="0"/>
+      <c r="AF2" s="0"/>
+      <c r="AG2" s="0"/>
+      <c r="AH2" s="0"/>
+      <c r="AI2" s="0"/>
+      <c r="AJ2" s="0"/>
+      <c r="AK2" s="0"/>
+      <c r="AL2" s="0"/>
+      <c r="AM2" s="0"/>
+      <c r="AN2" s="0"/>
+      <c r="AO2" s="0"/>
+      <c r="AP2" s="0"/>
+      <c r="AQ2" s="0"/>
+      <c r="AR2" s="0"/>
+      <c r="AS2" s="0"/>
+      <c r="AT2" s="0"/>
+      <c r="AU2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Customer class to interface with Excel spreadsheet
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
   <si>
     <t>First Name</t>
   </si>
@@ -65,42 +65,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>Barsoum</t>
-  </si>
-  <si>
-    <t>Yo</t>
-  </si>
-  <si>
-    <t>Hey</t>
-  </si>
-  <si>
-    <t>Wahba</t>
-  </si>
-  <si>
-    <t>Hatakalamina</t>
-  </si>
-  <si>
-    <t>Heyana</t>
-  </si>
-  <si>
-    <t>Likomi</t>
-  </si>
-  <si>
-    <t>Misaka</t>
-  </si>
-  <si>
-    <t>Jager</t>
-  </si>
-  <si>
-    <t>Arnold</t>
-  </si>
-  <si>
-    <t>Ackerman</t>
-  </si>
-  <si>
     <t>Room #</t>
   </si>
   <si>
@@ -108,45 +72,6 @@
   </si>
   <si>
     <t>Check Out</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>2024-01-10</t>
-  </si>
-  <si>
-    <t>2024-01-15</t>
-  </si>
-  <si>
-    <t>2024-02-20</t>
-  </si>
-  <si>
-    <t>2024-02-28</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>2024-01-20</t>
-  </si>
-  <si>
-    <t>2024-01-30</t>
-  </si>
-  <si>
-    <t>2023-01-10</t>
-  </si>
-  <si>
-    <t>2023-01-20</t>
   </si>
 </sst>
 </file>
@@ -1244,150 +1169,66 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="2"/>
   <sheetData>
-    <row r="1" customHeight="1" spans="2:17">
-      <c r="B1" t="s" s="0">
+    <row r="1" customHeight="1" spans="1:16">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s" s="0">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s" s="0">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s" s="0">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s" s="0">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s" s="0">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s" s="0">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s" s="0">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" customHeight="1" spans="1:4">
-      <c r="A2" s="0">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:3">
-      <c r="A3" s="0">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:3">
-      <c r="A4" s="0">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" customHeight="1" spans="1:3">
-      <c r="A5" s="0">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" customHeight="1" spans="1:3">
-      <c r="A6" s="0">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" customHeight="1" spans="1:3">
-      <c r="A7" s="0">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" customHeight="1" spans="1:1">
-      <c r="A8" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customHeight="1" spans="1:1">
-      <c r="A9" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customHeight="1" spans="1:1">
-      <c r="A10" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:1">
-      <c r="A11" s="0">
-        <v>10</v>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1397,141 +1238,151 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AI5"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="G1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="I1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="J1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="K1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="O1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="P1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="Q1" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="R1" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="S1" t="s" s="0">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="G2" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
-      <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
-      <c r="Q2" s="0"/>
-      <c r="R2" s="0"/>
-      <c r="S2" s="0"/>
-      <c r="T2" s="0"/>
-      <c r="U2" s="0"/>
-      <c r="V2" s="0"/>
-      <c r="W2" s="0"/>
-      <c r="X2" s="0"/>
-      <c r="Y2" s="0"/>
-      <c r="Z2" s="0"/>
-      <c r="AA2" s="0"/>
-      <c r="AB2" s="0"/>
-      <c r="AC2" s="0"/>
-      <c r="AD2" s="0"/>
-      <c r="AE2" s="0"/>
-      <c r="AF2" s="0"/>
-      <c r="AG2" s="0"/>
-      <c r="AH2" s="0"/>
-      <c r="AI2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>34</v>
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17">
+        <v>403</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated thank you page.
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -4,13 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="15975" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="Victims" sheetId="1" r:id="rId1"/>
     <sheet name="Rooms" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -77,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1169,13 +1182,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="1:16">
       <c r="A1" t="s">
@@ -1227,6 +1240,7 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1239,7 +1253,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Added documentation in JavaDoc style for classes and methods I worked on. Fixed a bug in the RoomSelection controller page. Deleted Room.java (deprecated and unused)
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -4,13 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="22410" windowHeight="10095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Victims" sheetId="1" r:id="rId1"/>
     <sheet name="Rooms" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -77,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1169,13 +1182,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="1:16">
       <c r="A1" t="s">
@@ -1227,6 +1240,7 @@
         <v>15</v>
       </c>
     </row>
+    <row r="2"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1238,8 +1252,8 @@
   <sheetPr/>
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
fixed exp month issue and total cost of stay
</commit_message>
<xml_diff>
--- a/The Phantom Inn.xlsx
+++ b/The Phantom Inn.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>First Name</t>
   </si>
@@ -85,6 +85,36 @@
   </si>
   <si>
     <t>Check Out</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>jdoe@gmail.com</t>
+  </si>
+  <si>
+    <t>3107957720</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>DOUBLE</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>2024-04-26</t>
+  </si>
+  <si>
+    <t>2024-04-28</t>
   </si>
 </sst>
 </file>
@@ -1191,56 +1221,81 @@
   <sheetFormatPr defaultColWidth="12.6285714285714" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <sheetData>
     <row r="1" customHeight="1" spans="1:16">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>15</v>
       </c>
     </row>
-    <row r="2"/>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1259,141 +1314,147 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" t="s" s="0">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>200</v>
       </c>
+      <c r="B6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>201</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>301</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>302</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>303</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>403</v>
       </c>
     </row>

</xml_diff>